<commit_message>
changes in TA repository for night shift
</commit_message>
<xml_diff>
--- a/ImillReports/Content/shift.xlsx
+++ b/ImillReports/Content/shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <x:si>
     <x:t>Employee Id</x:t>
   </x:si>
@@ -40,25 +40,13 @@
     <x:t>Late In</x:t>
   </x:si>
   <x:si>
-    <x:t>Zain Alaaabdin Hasan Mahmoud Alsayed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>العارضية</x:t>
-  </x:si>
-  <x:si>
-    <x:t>الادارة</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sahrukh Ahmedbhai Patel</x:t>
+    <x:t>Ibrahim Abu Aloyoun Kamel Mohammad</x:t>
   </x:si>
   <x:si>
     <x:t>Ardiya</x:t>
   </x:si>
   <x:si>
     <x:t>Not Punched</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ibrahim Abu Aloyoun Kamel Mohammad</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -416,7 +404,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H4"/>
+  <x:dimension ref="A1:H2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -450,7 +438,7 @@
     </x:row>
     <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>8</x:v>
@@ -458,65 +446,16 @@
       <x:c r="C2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
       <x:c r="E2" s="1" t="n">
         <x:v>0.916666666666667</x:v>
       </x:c>
       <x:c r="F2" s="1" t="n">
         <x:v>0.25</x:v>
       </x:c>
-      <x:c r="G2" s="1" t="n">
-        <x:v>0.430636574074074</x:v>
+      <x:c r="G2" s="0" t="s">
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H2" s="1" t="n">
-        <x:v>0.0139699074074074</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="0" t="n">
-        <x:v>169</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E3" s="1" t="n">
-        <x:v>0.916666666666667</x:v>
-      </x:c>
-      <x:c r="F3" s="1" t="n">
-        <x:v>0.25</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H3" s="1" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="0" t="n">
-        <x:v>162</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E4" s="1" t="n">
-        <x:v>0.916666666666667</x:v>
-      </x:c>
-      <x:c r="F4" s="1" t="n">
-        <x:v>0.25</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H4" s="1" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>